<commit_message>
Added icon handler and fix resize bug.
</commit_message>
<xml_diff>
--- a/TrafficSimulator/3Dobjects/3d_object_library.xlsx
+++ b/TrafficSimulator/3Dobjects/3d_object_library.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ELTE\Szakdoga\elte-ik-bsc-thesis\TrafficSimulator\3Dobjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495C5D37-16DF-479D-BF32-0A88EAC7F90E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5634392F-782C-44CC-AF52-D83E356CBACC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="825" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>little_car.obj</t>
   </si>
@@ -74,6 +74,24 @@
   </si>
   <si>
     <t>base</t>
+  </si>
+  <si>
+    <t>png</t>
+  </si>
+  <si>
+    <t>texture</t>
+  </si>
+  <si>
+    <t>default.png</t>
+  </si>
+  <si>
+    <t>road.png</t>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>icon.png</t>
   </si>
 </sst>
 </file>
@@ -932,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:AE4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,96 +977,129 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F4" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I4" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J4" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K4" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L4" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M4" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N4" t="s">
         <v>12</v>
       </c>
-      <c r="O1">
+      <c r="O4">
         <v>0</v>
       </c>
-      <c r="P1">
+      <c r="P4">
         <v>0</v>
       </c>
-      <c r="Q1">
+      <c r="Q4">
         <v>0</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R4" t="s">
         <v>13</v>
       </c>
-      <c r="S1">
+      <c r="S4">
         <v>1</v>
       </c>
-      <c r="T1">
+      <c r="T4">
         <v>1</v>
       </c>
-      <c r="U1">
+      <c r="U4">
         <v>1</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V4" t="s">
         <v>14</v>
       </c>
-      <c r="W1">
+      <c r="W4">
         <v>0</v>
       </c>
-      <c r="X1">
+      <c r="X4">
         <v>0</v>
       </c>
-      <c r="Y1">
+      <c r="Y4">
         <v>0</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z4" t="s">
         <v>15</v>
       </c>
-      <c r="AA1">
+      <c r="AA4">
         <v>0</v>
       </c>
-      <c r="AB1">
+      <c r="AB4">
         <v>0</v>
       </c>
-      <c r="AC1">
+      <c r="AC4">
         <v>0</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD4" t="s">
         <v>16</v>
       </c>
-      <c r="AE1">
+      <c r="AE4">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto object loader working.
</commit_message>
<xml_diff>
--- a/TrafficSimulator/3Dobjects/3d_object_library.xlsx
+++ b/TrafficSimulator/3Dobjects/3d_object_library.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ELTE\Szakdoga\elte-ik-bsc-thesis\TrafficSimulator\3Dobjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5634392F-782C-44CC-AF52-D83E356CBACC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB4D7FC-59A6-4915-8368-C7A49F9CEDE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="825" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t>little_car.obj</t>
   </si>
@@ -34,24 +34,9 @@
     <t>little_car_red_break.png</t>
   </si>
   <si>
-    <t>obj</t>
-  </si>
-  <si>
-    <t>break</t>
-  </si>
-  <si>
-    <t>light</t>
-  </si>
-  <si>
     <t>little_car_red_light.png</t>
   </si>
   <si>
-    <t>right</t>
-  </si>
-  <si>
-    <t>left</t>
-  </si>
-  <si>
     <t>little_car_red_left.png</t>
   </si>
   <si>
@@ -73,12 +58,6 @@
     <t>hitSphereSize</t>
   </si>
   <si>
-    <t>base</t>
-  </si>
-  <si>
-    <t>png</t>
-  </si>
-  <si>
     <t>texture</t>
   </si>
   <si>
@@ -91,7 +70,82 @@
     <t>icon</t>
   </si>
   <si>
-    <t>icon.png</t>
+    <t>little_car_blue_base.png</t>
+  </si>
+  <si>
+    <t>little_car_blue_light.png</t>
+  </si>
+  <si>
+    <t>little_car_blue_break.png</t>
+  </si>
+  <si>
+    <t>little_car_blue_right.png</t>
+  </si>
+  <si>
+    <t>little_car_blue_left.png</t>
+  </si>
+  <si>
+    <t>little_car_green_base.png</t>
+  </si>
+  <si>
+    <t>little_car_green_light.png</t>
+  </si>
+  <si>
+    <t>little_car_green_break.png</t>
+  </si>
+  <si>
+    <t>little_car_green_right.png</t>
+  </si>
+  <si>
+    <t>little_car_green_left.png</t>
+  </si>
+  <si>
+    <t>Little red car</t>
+  </si>
+  <si>
+    <t>Little green car</t>
+  </si>
+  <si>
+    <t>app_icon.png</t>
+  </si>
+  <si>
+    <t>Default texture</t>
+  </si>
+  <si>
+    <t>Road texture</t>
+  </si>
+  <si>
+    <t>app_logo.png</t>
+  </si>
+  <si>
+    <t>Logo</t>
+  </si>
+  <si>
+    <t>Icon</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Main object</t>
+  </si>
+  <si>
+    <t>base texture</t>
+  </si>
+  <si>
+    <t>light texture</t>
+  </si>
+  <si>
+    <t>break texture</t>
+  </si>
+  <si>
+    <t>right texture</t>
+  </si>
+  <si>
+    <t>left texture</t>
   </si>
 </sst>
 </file>
@@ -593,8 +647,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - 1. jelölőszín" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -950,160 +1007,330 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE4"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.85546875" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
-    <col min="4" max="4" width="7.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.5703125" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" customWidth="1"/>
-    <col min="8" max="8" width="7.7109375" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" customWidth="1"/>
-    <col min="13" max="13" width="22" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" customWidth="1"/>
-    <col min="18" max="18" width="8.5703125" customWidth="1"/>
-    <col min="22" max="22" width="11.5703125" customWidth="1"/>
-    <col min="26" max="26" width="17.5703125" customWidth="1"/>
-    <col min="30" max="30" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="22.5703125" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="3.7109375" customWidth="1"/>
+    <col min="10" max="10" width="4.28515625" customWidth="1"/>
+    <col min="11" max="11" width="3.85546875" customWidth="1"/>
+    <col min="12" max="13" width="3.42578125" customWidth="1"/>
+    <col min="14" max="14" width="4.140625" customWidth="1"/>
+    <col min="15" max="15" width="3.42578125" customWidth="1"/>
+    <col min="16" max="16" width="3.7109375" customWidth="1"/>
+    <col min="17" max="17" width="3.5703125" customWidth="1"/>
+    <col min="18" max="18" width="6.28515625" customWidth="1"/>
+    <col min="19" max="19" width="6.5703125" customWidth="1"/>
+    <col min="20" max="20" width="5.7109375" customWidth="1"/>
+    <col min="21" max="21" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="H7" t="s">
         <v>20</v>
       </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="E8" t="s">
         <v>22</v>
       </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="F8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" t="s">
-        <v>5</v>
-      </c>
-      <c r="I4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" t="s">
-        <v>9</v>
-      </c>
-      <c r="M4" t="s">
-        <v>10</v>
-      </c>
-      <c r="N4" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4" t="s">
-        <v>13</v>
-      </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-      <c r="T4">
-        <v>1</v>
-      </c>
-      <c r="U4">
-        <v>1</v>
-      </c>
-      <c r="V4" t="s">
-        <v>14</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
-      </c>
-      <c r="Y4">
-        <v>0</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA4">
-        <v>0</v>
-      </c>
-      <c r="AB4">
-        <v>0</v>
-      </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE4">
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
+      </c>
+      <c r="U8">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="R1:T1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Paralel opengl texture loader working.
</commit_message>
<xml_diff>
--- a/TrafficSimulator/3Dobjects/3d_object_library.xlsx
+++ b/TrafficSimulator/3Dobjects/3d_object_library.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ELTE\Szakdoga\elte-ik-bsc-thesis\TrafficSimulator\3Dobjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EB4D7FC-59A6-4915-8368-C7A49F9CEDE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B74CD74A-C50C-48E3-913F-5D120FFE7756}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="825" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1010,7 +1010,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
ObjectAdding and move is working
</commit_message>
<xml_diff>
--- a/TrafficSimulator/3Dobjects/3d_object_library.xlsx
+++ b/TrafficSimulator/3Dobjects/3d_object_library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ELTE\Szakdoga\elte-ik-bsc-thesis\TrafficSimulator\3Dobjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{50E409F1-8496-44B8-A5B2-D712BB73650C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1F427CA-9F72-418D-A954-1DA2BA09C1B4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3d_object_library" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="148">
   <si>
     <t>little_car.obj</t>
   </si>
@@ -455,6 +455,15 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>FirstCene</t>
+  </si>
+  <si>
+    <t>desk</t>
+  </si>
+  <si>
+    <t>mark</t>
   </si>
 </sst>
 </file>
@@ -977,10 +986,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1338,10 +1347,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF28"/>
+  <dimension ref="A1:AG28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1371,108 +1380,114 @@
     <col min="24" max="24" width="13.140625" style="1" customWidth="1"/>
     <col min="25" max="27" width="9.140625" style="1"/>
     <col min="28" max="28" width="16.42578125" style="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="1"/>
+    <col min="29" max="32" width="9.140625" style="1"/>
+    <col min="33" max="33" width="9.7109375" style="1" customWidth="1"/>
+    <col min="34" max="34" width="12.140625" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5">
+    <row r="1" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4">
         <v>0</v>
       </c>
-      <c r="B1" s="5">
+      <c r="B1" s="4">
         <v>1</v>
       </c>
-      <c r="C1" s="5">
+      <c r="C1" s="4">
         <v>2</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1" s="4">
         <v>3</v>
       </c>
-      <c r="E1" s="5">
+      <c r="E1" s="4">
         <v>4</v>
       </c>
-      <c r="F1" s="5">
+      <c r="F1" s="4">
         <v>5</v>
       </c>
-      <c r="G1" s="5">
+      <c r="G1" s="4">
         <v>6</v>
       </c>
-      <c r="H1" s="5">
+      <c r="H1" s="4">
         <v>7</v>
       </c>
-      <c r="I1" s="5">
+      <c r="I1" s="4">
         <v>8</v>
       </c>
-      <c r="J1" s="5">
+      <c r="J1" s="4">
         <v>9</v>
       </c>
-      <c r="K1" s="5">
+      <c r="K1" s="4">
         <v>10</v>
       </c>
-      <c r="L1" s="5">
+      <c r="L1" s="4">
         <v>11</v>
       </c>
-      <c r="M1" s="5">
+      <c r="M1" s="4">
         <v>12</v>
       </c>
-      <c r="N1" s="5">
+      <c r="N1" s="4">
         <v>13</v>
       </c>
-      <c r="O1" s="5">
+      <c r="O1" s="4">
         <v>14</v>
       </c>
-      <c r="P1" s="5">
+      <c r="P1" s="4">
         <v>15</v>
       </c>
-      <c r="Q1" s="5">
+      <c r="Q1" s="4">
         <v>16</v>
       </c>
-      <c r="R1" s="5">
+      <c r="R1" s="4">
         <v>17</v>
       </c>
-      <c r="S1" s="5">
+      <c r="S1" s="4">
         <v>18</v>
       </c>
-      <c r="T1" s="5">
+      <c r="T1" s="4">
         <v>19</v>
       </c>
-      <c r="U1" s="5">
+      <c r="U1" s="4">
         <v>20</v>
       </c>
-      <c r="V1" s="5">
+      <c r="V1" s="4">
         <v>21</v>
       </c>
-      <c r="W1" s="5">
+      <c r="W1" s="4">
         <v>22</v>
       </c>
-      <c r="X1" s="5">
+      <c r="X1" s="4">
         <v>23</v>
       </c>
-      <c r="Y1" s="5">
+      <c r="Y1" s="4">
         <v>24</v>
       </c>
-      <c r="Z1" s="5">
+      <c r="Z1" s="4">
         <v>25</v>
       </c>
-      <c r="AA1" s="5">
+      <c r="AA1" s="4">
         <v>26</v>
       </c>
-      <c r="AB1" s="5">
+      <c r="AB1" s="4">
         <v>27</v>
       </c>
-      <c r="AC1" s="5">
+      <c r="AC1" s="4">
         <v>28</v>
       </c>
-      <c r="AD1" s="5">
+      <c r="AD1" s="4">
         <v>29</v>
       </c>
-      <c r="AE1" s="5">
+      <c r="AE1" s="4">
         <v>30</v>
       </c>
-      <c r="AF1" s="5">
+      <c r="AF1" s="4">
         <v>31</v>
       </c>
+      <c r="AG1" s="4">
+        <v>32</v>
+      </c>
     </row>
-    <row r="2" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>130</v>
       </c>
@@ -1503,35 +1518,35 @@
       <c r="J2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4" t="s">
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4" t="s">
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="4"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4" t="s">
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
       <c r="X2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
       <c r="AB2" s="3" t="s">
         <v>116</v>
       </c>
@@ -1547,8 +1562,11 @@
       <c r="AF2" s="3" t="s">
         <v>128</v>
       </c>
+      <c r="AG2" s="3" t="s">
+        <v>145</v>
+      </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>-1</v>
       </c>
@@ -1645,8 +1663,11 @@
       <c r="AF3" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="AG3" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>-1</v>
       </c>
@@ -1743,8 +1764,11 @@
       <c r="AF4" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="AG4" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>-1</v>
       </c>
@@ -1841,8 +1865,11 @@
       <c r="AF5" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="AG5" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>-1</v>
       </c>
@@ -1939,8 +1966,11 @@
       <c r="AF6" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="AG6" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -1948,7 +1978,7 @@
         <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>41</v>
+        <v>147</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>51</v>
@@ -2037,8 +2067,11 @@
       <c r="AF7" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG7" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -2135,8 +2168,11 @@
       <c r="AF8" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG8" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -2233,8 +2269,11 @@
       <c r="AF9" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG9" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -2242,7 +2281,7 @@
         <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>41</v>
+        <v>146</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>45</v>
@@ -2331,8 +2370,11 @@
       <c r="AF10" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG10" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>5</v>
       </c>
@@ -2340,7 +2382,7 @@
         <v>47</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>41</v>
+        <v>146</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>48</v>
@@ -2429,8 +2471,11 @@
       <c r="AF11" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG11" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -2527,8 +2572,11 @@
       <c r="AF12" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG12" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>7</v>
       </c>
@@ -2625,8 +2673,11 @@
       <c r="AF13" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG13" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>8</v>
       </c>
@@ -2723,8 +2774,11 @@
       <c r="AF14" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG14" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>9</v>
       </c>
@@ -2821,8 +2875,11 @@
       <c r="AF15" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG15" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>10</v>
       </c>
@@ -2919,8 +2976,11 @@
       <c r="AF16" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG16" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>11</v>
       </c>
@@ -3017,8 +3077,11 @@
       <c r="AF17" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG17" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>12</v>
       </c>
@@ -3115,8 +3178,11 @@
       <c r="AF18" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG18" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>13</v>
       </c>
@@ -3213,8 +3279,11 @@
       <c r="AF19" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG19" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>14</v>
       </c>
@@ -3311,8 +3380,11 @@
       <c r="AF20" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG20" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>15</v>
       </c>
@@ -3409,8 +3481,11 @@
       <c r="AF21" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG21" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>16</v>
       </c>
@@ -3507,8 +3582,11 @@
       <c r="AF22" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG22" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>17</v>
       </c>
@@ -3605,8 +3683,11 @@
       <c r="AF23" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG23" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>18</v>
       </c>
@@ -3703,8 +3784,11 @@
       <c r="AF24" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG24" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>19</v>
       </c>
@@ -3801,8 +3885,11 @@
       <c r="AF25" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG25" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>20</v>
       </c>
@@ -3899,8 +3986,11 @@
       <c r="AF26" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG26" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>21</v>
       </c>
@@ -3997,8 +4087,11 @@
       <c r="AF27" s="1" t="s">
         <v>107</v>
       </c>
+      <c r="AG27" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>22</v>
       </c>
@@ -4094,6 +4187,9 @@
       </c>
       <c r="AF28" s="1" t="s">
         <v>107</v>
+      </c>
+      <c r="AG28" s="1" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Texture glitch and anti aliasing problem solved.
</commit_message>
<xml_diff>
--- a/TrafficSimulator/3Dobjects/3d_object_library.xlsx
+++ b/TrafficSimulator/3Dobjects/3d_object_library.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ELTE\Szakdoga\elte-ik-bsc-thesis\TrafficSimulator\3Dobjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA71212-4448-495C-91B7-5F32B6CC39AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01090510-CC39-45E9-A6E4-DB988FF39B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="825" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1349,8 +1349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7:T7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2011,13 +2011,13 @@
         <v>105</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="Q7" s="1" t="s">
         <v>105</v>
@@ -2041,7 +2041,7 @@
         <v>105</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>107</v>
+        <v>117</v>
       </c>
       <c r="Y7" s="1" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
Road round endings and road bugfix
</commit_message>
<xml_diff>
--- a/TrafficSimulator/3Dobjects/3d_object_library.xlsx
+++ b/TrafficSimulator/3Dobjects/3d_object_library.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ELTE\Szakdoga\elte-ik-bsc-thesis\TrafficSimulator\3Dobjects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandorbalazs\Desktop\elte-ik-bsc-thesis\TrafficSimulator\3Dobjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01090510-CC39-45E9-A6E4-DB988FF39B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6846F68C-B795-404F-B9AC-028D5777DB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3d_object_library" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="153">
   <si>
     <t>little_car.obj</t>
   </si>
@@ -464,6 +464,21 @@
   </si>
   <si>
     <t>mark</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>Road circle</t>
+  </si>
+  <si>
+    <t>road_circle.obj</t>
+  </si>
+  <si>
+    <t>road_circle.png</t>
+  </si>
+  <si>
+    <t>2.0</t>
   </si>
 </sst>
 </file>
@@ -1347,46 +1362,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG28"/>
+  <dimension ref="A1:AG29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="21.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="25.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="30.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="29.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="30.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="30.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="31.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="21.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="1"/>
+    <col min="4" max="4" width="25.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="30.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="29.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="30.88671875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="31.33203125" style="1" customWidth="1"/>
     <col min="11" max="11" width="5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="5.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="5.33203125" style="1" customWidth="1"/>
     <col min="13" max="13" width="5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="4.42578125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="4.5703125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="4.44140625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="4.5546875" style="1" customWidth="1"/>
     <col min="16" max="17" width="5" style="1" customWidth="1"/>
-    <col min="18" max="18" width="4.7109375" style="1" customWidth="1"/>
-    <col min="19" max="19" width="4.5703125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="4.28515625" style="1" customWidth="1"/>
-    <col min="21" max="21" width="6.28515625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="6.5703125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="5.7109375" style="1" customWidth="1"/>
-    <col min="24" max="24" width="13.140625" style="1" customWidth="1"/>
-    <col min="25" max="27" width="9.140625" style="1"/>
-    <col min="28" max="28" width="16.42578125" style="1" customWidth="1"/>
-    <col min="29" max="32" width="9.140625" style="1"/>
-    <col min="33" max="33" width="9.7109375" style="1" customWidth="1"/>
-    <col min="34" max="34" width="12.140625" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="1"/>
+    <col min="18" max="18" width="4.6640625" style="1" customWidth="1"/>
+    <col min="19" max="19" width="4.5546875" style="1" customWidth="1"/>
+    <col min="20" max="20" width="4.33203125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="6.33203125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="6.5546875" style="1" customWidth="1"/>
+    <col min="23" max="23" width="5.6640625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="13.109375" style="1" customWidth="1"/>
+    <col min="25" max="27" width="9.109375" style="1"/>
+    <col min="28" max="28" width="16.44140625" style="1" customWidth="1"/>
+    <col min="29" max="32" width="9.109375" style="1"/>
+    <col min="33" max="33" width="9.6640625" style="1" customWidth="1"/>
+    <col min="34" max="34" width="12.109375" style="1" customWidth="1"/>
+    <col min="35" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4">
         <v>0</v>
       </c>
@@ -1487,7 +1502,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>130</v>
       </c>
@@ -1566,7 +1581,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>-1</v>
       </c>
@@ -1667,7 +1682,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>-1</v>
       </c>
@@ -1768,7 +1783,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>-1</v>
       </c>
@@ -1869,7 +1884,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>-1</v>
       </c>
@@ -1970,7 +1985,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -2071,7 +2086,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -2172,7 +2187,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -2273,7 +2288,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -2374,7 +2389,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>5</v>
       </c>
@@ -2475,7 +2490,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -2576,7 +2591,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>7</v>
       </c>
@@ -2677,7 +2692,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>8</v>
       </c>
@@ -2778,7 +2793,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>9</v>
       </c>
@@ -2879,7 +2894,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>10</v>
       </c>
@@ -2980,7 +2995,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>11</v>
       </c>
@@ -3081,7 +3096,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>12</v>
       </c>
@@ -3182,7 +3197,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>13</v>
       </c>
@@ -3283,7 +3298,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>14</v>
       </c>
@@ -3384,7 +3399,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>15</v>
       </c>
@@ -3485,7 +3500,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>16</v>
       </c>
@@ -3586,7 +3601,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>17</v>
       </c>
@@ -3687,7 +3702,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>18</v>
       </c>
@@ -3788,7 +3803,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>19</v>
       </c>
@@ -3889,7 +3904,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>20</v>
       </c>
@@ -3990,7 +4005,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>21</v>
       </c>
@@ -4091,7 +4106,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>22</v>
       </c>
@@ -4189,6 +4204,107 @@
         <v>107</v>
       </c>
       <c r="AG28" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="T29" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="U29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="W29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="X29" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA29" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB29" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AC29" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD29" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE29" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF29" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG29" s="1" t="s">
         <v>143</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding start and finish signs.
</commit_message>
<xml_diff>
--- a/TrafficSimulator/3Dobjects/3d_object_library.xlsx
+++ b/TrafficSimulator/3Dobjects/3d_object_library.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandorbalazs\Desktop\elte-ik-bsc-thesis\TrafficSimulator\3Dobjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6846F68C-B795-404F-B9AC-028D5777DB3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CE9C118-757B-4678-B25A-195952111B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="887" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="160">
   <si>
     <t>little_car.obj</t>
   </si>
@@ -479,6 +479,27 @@
   </si>
   <si>
     <t>2.0</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>Start sign</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Stop sign</t>
+  </si>
+  <si>
+    <t>sign.obj</t>
+  </si>
+  <si>
+    <t>start_sign.png</t>
+  </si>
+  <si>
+    <t>stop_sign.png</t>
   </si>
 </sst>
 </file>
@@ -1362,10 +1383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG29"/>
+  <dimension ref="A1:AG31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4308,6 +4329,208 @@
         <v>143</v>
       </c>
     </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="R30" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="T30" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="U30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="W30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="X30" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB30" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AC30" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD30" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE30" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF30" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG30" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="T31" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="U31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="W31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="X31" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="Y31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB31" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AC31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AD31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG31" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="K2:M2"/>

</xml_diff>

<commit_message>
Documentation. GUI development and new textures and positions.
</commit_message>
<xml_diff>
--- a/TrafficSimulator/3Dobjects/3d_object_library.xlsx
+++ b/TrafficSimulator/3Dobjects/3d_object_library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandorbalazs\Desktop\elte-ik-bsc-thesis\TrafficSimulator\3Dobjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0106B3E-4733-4BA0-8220-EA24E70C64EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{366B1AE1-7683-453A-818F-BC9CB8F7A7AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3d_object_library" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="178">
   <si>
     <t>little_car.obj</t>
   </si>
@@ -548,6 +548,12 @@
   </si>
   <si>
     <t>delete_mini.png</t>
+  </si>
+  <si>
+    <t>20.0</t>
+  </si>
+  <si>
+    <t>55.0</t>
   </si>
 </sst>
 </file>
@@ -1436,8 +1442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2196,7 +2202,7 @@
         <v>105</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>105</v>
+        <v>176</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>116</v>
@@ -3806,7 +3812,7 @@
         <v>42</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>105</v>
+        <v>177</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>105</v>
@@ -3907,7 +3913,7 @@
         <v>42</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>105</v>
+        <v>177</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>105</v>
@@ -4008,7 +4014,7 @@
         <v>42</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>105</v>
+        <v>177</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>105</v>
@@ -4109,7 +4115,7 @@
         <v>42</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>105</v>
+        <v>177</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>105</v>
@@ -4210,7 +4216,7 @@
         <v>42</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>105</v>
+        <v>177</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>105</v>
@@ -4311,7 +4317,7 @@
         <v>42</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>105</v>
+        <v>177</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>105</v>
@@ -4412,7 +4418,7 @@
         <v>42</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>105</v>
+        <v>177</v>
       </c>
       <c r="L30" s="1" t="s">
         <v>105</v>
@@ -4513,7 +4519,7 @@
         <v>42</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>105</v>
+        <v>177</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>105</v>
@@ -4614,7 +4620,7 @@
         <v>42</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>105</v>
+        <v>177</v>
       </c>
       <c r="L32" s="1" t="s">
         <v>105</v>
@@ -4715,7 +4721,7 @@
         <v>42</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>105</v>
+        <v>177</v>
       </c>
       <c r="L33" s="1" t="s">
         <v>105</v>
@@ -4816,7 +4822,7 @@
         <v>42</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>105</v>
+        <v>177</v>
       </c>
       <c r="L34" s="1" t="s">
         <v>105</v>
@@ -4917,7 +4923,7 @@
         <v>42</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>105</v>
+        <v>177</v>
       </c>
       <c r="L35" s="1" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
Finalizing and vehicle select.
</commit_message>
<xml_diff>
--- a/TrafficSimulator/3Dobjects/3d_object_library.xlsx
+++ b/TrafficSimulator/3Dobjects/3d_object_library.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandorbalazs\Desktop\elte-ik-bsc-thesis\TrafficSimulator\3Dobjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CED66F7-CCAF-4787-BB43-845EAA80F5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56032FB1-5D94-4440-9B3F-90B517BCB7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3d_object_library" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="181">
   <si>
     <t>little_car.obj</t>
   </si>
@@ -560,6 +560,9 @@
   </si>
   <si>
     <t>controls.png</t>
+  </si>
+  <si>
+    <t>0.1</t>
   </si>
 </sst>
 </file>
@@ -1448,8 +1451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2443,7 +2446,7 @@
         <v>105</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="Y10" s="1" t="s">
         <v>105</v>

</xml_diff>

<commit_message>
GUI upgrade, statistics and road coloring menu.
</commit_message>
<xml_diff>
--- a/TrafficSimulator/3Dobjects/3d_object_library.xlsx
+++ b/TrafficSimulator/3Dobjects/3d_object_library.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandorbalazs\Desktop\elte-ik-bsc-thesis\TrafficSimulator\3Dobjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CCD901-DD21-487C-8EF8-516D94D8B71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0E3149-2EC4-4CB0-A2C7-B2435A1EBC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="185">
   <si>
     <t>little_car.obj</t>
   </si>
@@ -563,6 +563,18 @@
   </si>
   <si>
     <t>-0.5</t>
+  </si>
+  <si>
+    <t>Bundus</t>
+  </si>
+  <si>
+    <t>bundus.png</t>
+  </si>
+  <si>
+    <t>ELTE</t>
+  </si>
+  <si>
+    <t>elte.png</t>
   </si>
 </sst>
 </file>
@@ -1449,10 +1461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG36"/>
+  <dimension ref="A1:AG38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2178,13 +2190,13 @@
         <v>-1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>42</v>
@@ -2275,23 +2287,23 @@
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A9" s="6">
-        <v>1</v>
+      <c r="A9" s="5">
+        <v>-1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>52</v>
+        <v>183</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>145</v>
+        <v>12</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>51</v>
+        <v>184</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>42</v>
@@ -2306,93 +2318,93 @@
         <v>42</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>175</v>
+        <v>42</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>142</v>
+        <v>42</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="Z9" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>122</v>
+        <v>42</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AD9" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AE9" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AF9" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AG9" s="1" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
-        <v>2</v>
+      <c r="A10" s="5">
+        <v>-1</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>146</v>
+        <v>177</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>145</v>
+        <v>12</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>147</v>
+        <v>178</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>148</v>
+        <v>42</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>42</v>
@@ -2407,70 +2419,70 @@
         <v>42</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>142</v>
+        <v>42</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="V10" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="W10" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>179</v>
+        <v>42</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="Z10" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>149</v>
+        <v>42</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AD10" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AE10" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AF10" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AG10" s="1" t="s">
         <v>141</v>
@@ -2478,22 +2490,22 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>42</v>
@@ -2510,20 +2522,20 @@
       <c r="K11" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L11" s="2" t="s">
-        <v>112</v>
+      <c r="L11" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>105</v>
+        <v>175</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="Q11" s="1" t="s">
         <v>105</v>
@@ -2547,7 +2559,7 @@
         <v>105</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="Y11" s="1" t="s">
         <v>105</v>
@@ -2559,7 +2571,7 @@
         <v>105</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="AC11" s="1" t="s">
         <v>106</v>
@@ -2579,22 +2591,22 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>146</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>48</v>
+        <v>147</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>99</v>
+        <v>42</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>49</v>
+        <v>148</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>42</v>
@@ -2611,20 +2623,20 @@
       <c r="K12" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L12" s="2" t="s">
-        <v>112</v>
+      <c r="L12" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>105</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="Q12" s="1" t="s">
         <v>105</v>
@@ -2648,7 +2660,7 @@
         <v>105</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>111</v>
+        <v>179</v>
       </c>
       <c r="Y12" s="1" t="s">
         <v>105</v>
@@ -2660,7 +2672,7 @@
         <v>105</v>
       </c>
       <c r="AB12" s="1" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="AC12" s="1" t="s">
         <v>106</v>
@@ -2675,57 +2687,57 @@
         <v>106</v>
       </c>
       <c r="AG12" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" s="6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L13" s="1" t="s">
-        <v>105</v>
+      <c r="L13" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="M13" s="1" t="s">
         <v>105</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="Q13" s="1" t="s">
         <v>105</v>
@@ -2749,19 +2761,19 @@
         <v>105</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y13" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="Y13" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="AA13" s="1" t="s">
         <v>105</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="AC13" s="1" t="s">
         <v>106</v>
@@ -2781,52 +2793,52 @@
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>130</v>
+        <v>99</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>16</v>
+        <v>49</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L14" s="1" t="s">
-        <v>105</v>
+      <c r="L14" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="M14" s="1" t="s">
         <v>105</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>105</v>
@@ -2850,19 +2862,19 @@
         <v>105</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y14" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="Y14" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="AA14" s="1" t="s">
         <v>105</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="AC14" s="1" t="s">
         <v>106</v>
@@ -2877,15 +2889,15 @@
         <v>106</v>
       </c>
       <c r="AG14" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" s="6">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>1</v>
@@ -2894,22 +2906,22 @@
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>105</v>
@@ -2983,34 +2995,34 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>53</v>
+        <v>20</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>105</v>
@@ -3043,7 +3055,7 @@
         <v>141</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>180</v>
+        <v>105</v>
       </c>
       <c r="V16" s="1" t="s">
         <v>105</v>
@@ -3054,8 +3066,8 @@
       <c r="X16" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="Y16" s="1" t="s">
-        <v>105</v>
+      <c r="Y16" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="Z16" s="1" t="s">
         <v>109</v>
@@ -3084,34 +3096,34 @@
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" s="6">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>105</v>
@@ -3144,7 +3156,7 @@
         <v>141</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>180</v>
+        <v>105</v>
       </c>
       <c r="V17" s="1" t="s">
         <v>105</v>
@@ -3155,8 +3167,8 @@
       <c r="X17" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="Y17" s="1" t="s">
-        <v>105</v>
+      <c r="Y17" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="Z17" s="1" t="s">
         <v>109</v>
@@ -3185,10 +3197,10 @@
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>1</v>
@@ -3197,22 +3209,22 @@
         <v>50</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>105</v>
@@ -3286,34 +3298,34 @@
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" s="6">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>105</v>
@@ -3346,7 +3358,7 @@
         <v>141</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>105</v>
+        <v>180</v>
       </c>
       <c r="V19" s="1" t="s">
         <v>105</v>
@@ -3355,19 +3367,19 @@
         <v>105</v>
       </c>
       <c r="X19" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y19" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
+      </c>
+      <c r="Y19" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="Z19" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="AA19" s="1" t="s">
         <v>105</v>
       </c>
       <c r="AB19" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="AC19" s="1" t="s">
         <v>106</v>
@@ -3387,34 +3399,34 @@
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>105</v>
@@ -3447,7 +3459,7 @@
         <v>141</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>105</v>
+        <v>180</v>
       </c>
       <c r="V20" s="1" t="s">
         <v>105</v>
@@ -3456,19 +3468,19 @@
         <v>105</v>
       </c>
       <c r="X20" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y20" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
+      </c>
+      <c r="Y20" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="Z20" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="AA20" s="1" t="s">
         <v>105</v>
       </c>
       <c r="AB20" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="AC20" s="1" t="s">
         <v>106</v>
@@ -3488,10 +3500,10 @@
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" s="6">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>1</v>
@@ -3500,22 +3512,22 @@
         <v>69</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>105</v>
@@ -3589,34 +3601,34 @@
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>105</v>
@@ -3660,11 +3672,11 @@
       <c r="X22" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="Y22" s="1" t="s">
-        <v>105</v>
+      <c r="Y22" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="Z22" s="1" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="AA22" s="1" t="s">
         <v>105</v>
@@ -3690,34 +3702,34 @@
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" s="6">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>105</v>
@@ -3761,11 +3773,11 @@
       <c r="X23" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="Y23" s="1" t="s">
-        <v>105</v>
+      <c r="Y23" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="Z23" s="1" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="AA23" s="1" t="s">
         <v>105</v>
@@ -3791,10 +3803,10 @@
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>1</v>
@@ -3803,22 +3815,22 @@
         <v>73</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>105</v>
@@ -3892,37 +3904,37 @@
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" s="6">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>150</v>
+        <v>78</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>152</v>
+        <v>73</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>153</v>
+        <v>76</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
       <c r="L25" s="1" t="s">
         <v>105</v>
@@ -3931,13 +3943,13 @@
         <v>105</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Q25" s="1" t="s">
         <v>105</v>
@@ -3961,19 +3973,19 @@
         <v>105</v>
       </c>
       <c r="X25" s="1" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
       <c r="Y25" s="1" t="s">
         <v>105</v>
       </c>
       <c r="Z25" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AA25" s="1" t="s">
         <v>105</v>
       </c>
       <c r="AB25" s="1" t="s">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="AC25" s="1" t="s">
         <v>106</v>
@@ -3993,37 +4005,37 @@
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26" s="7">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>152</v>
+        <v>73</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>154</v>
+        <v>75</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
       <c r="L26" s="1" t="s">
         <v>105</v>
@@ -4032,13 +4044,13 @@
         <v>105</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Q26" s="1" t="s">
         <v>105</v>
@@ -4062,19 +4074,19 @@
         <v>105</v>
       </c>
       <c r="X26" s="1" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
       <c r="Y26" s="1" t="s">
         <v>105</v>
       </c>
       <c r="Z26" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AA26" s="1" t="s">
         <v>105</v>
       </c>
       <c r="AB26" s="1" t="s">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="AC26" s="1" t="s">
         <v>106</v>
@@ -4094,22 +4106,22 @@
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" s="6">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>79</v>
+        <v>150</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>80</v>
+        <v>152</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>100</v>
+        <v>160</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>81</v>
+        <v>153</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>42</v>
@@ -4133,13 +4145,13 @@
         <v>105</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>108</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q27" s="1" t="s">
         <v>105</v>
@@ -4163,7 +4175,7 @@
         <v>105</v>
       </c>
       <c r="X27" s="1" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="Y27" s="1" t="s">
         <v>105</v>
@@ -4175,7 +4187,7 @@
         <v>105</v>
       </c>
       <c r="AB27" s="1" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="AC27" s="1" t="s">
         <v>106</v>
@@ -4195,22 +4207,22 @@
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28" s="7">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>83</v>
+        <v>151</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>101</v>
+        <v>161</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>84</v>
+        <v>154</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>42</v>
@@ -4234,13 +4246,13 @@
         <v>105</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O28" s="1" t="s">
         <v>108</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q28" s="1" t="s">
         <v>105</v>
@@ -4264,7 +4276,7 @@
         <v>105</v>
       </c>
       <c r="X28" s="1" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="Y28" s="1" t="s">
         <v>105</v>
@@ -4276,7 +4288,7 @@
         <v>105</v>
       </c>
       <c r="AB28" s="1" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="AC28" s="1" t="s">
         <v>106</v>
@@ -4296,22 +4308,22 @@
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A29" s="6">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>42</v>
@@ -4397,22 +4409,22 @@
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30" s="7">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>42</v>
@@ -4498,22 +4510,22 @@
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A31" s="6">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>42</v>
@@ -4599,22 +4611,22 @@
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>42</v>
@@ -4638,13 +4650,13 @@
         <v>105</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>166</v>
+        <v>107</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>166</v>
+        <v>108</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>166</v>
+        <v>109</v>
       </c>
       <c r="Q32" s="1" t="s">
         <v>105</v>
@@ -4700,22 +4712,22 @@
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A33" s="6">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>63</v>
+        <v>91</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>64</v>
+        <v>92</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>42</v>
@@ -4739,13 +4751,13 @@
         <v>105</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>171</v>
+        <v>107</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>171</v>
+        <v>109</v>
       </c>
       <c r="Q33" s="1" t="s">
         <v>105</v>
@@ -4801,22 +4813,22 @@
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>159</v>
+        <v>60</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>155</v>
+        <v>61</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>167</v>
+        <v>96</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>42</v>
@@ -4840,13 +4852,13 @@
         <v>105</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="Q34" s="1" t="s">
         <v>105</v>
@@ -4902,22 +4914,22 @@
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A35" s="6">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>157</v>
+        <v>63</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>156</v>
+        <v>64</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>168</v>
+        <v>97</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>163</v>
+        <v>65</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>42</v>
@@ -4941,13 +4953,13 @@
         <v>105</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="Q35" s="1" t="s">
         <v>105</v>
@@ -5003,22 +5015,22 @@
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>42</v>
@@ -5042,13 +5054,13 @@
         <v>105</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="Q36" s="1" t="s">
         <v>105</v>
@@ -5099,6 +5111,208 @@
         <v>106</v>
       </c>
       <c r="AG36" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A37" s="6">
+        <v>27</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="L37" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="O37" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="P37" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q37" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="R37" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="S37" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="U37" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V37" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="W37" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="X37" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y37" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z37" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA37" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB37" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC37" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD37" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE37" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF37" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG37" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A38" s="7">
+        <v>28</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N38" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="P38" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="R38" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="S38" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="T38" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="U38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="W38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="X38" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB38" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC38" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD38" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE38" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF38" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG38" s="1" t="s">
         <v>141</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding HELP window content.
</commit_message>
<xml_diff>
--- a/TrafficSimulator/3Dobjects/3d_object_library.xlsx
+++ b/TrafficSimulator/3Dobjects/3d_object_library.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandorbalazs\Desktop\elte-ik-bsc-thesis\TrafficSimulator\3Dobjects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0E3149-2EC4-4CB0-A2C7-B2435A1EBC02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C16131-67DB-4AD5-B47E-B7C53971C4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1174" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1270" uniqueCount="191">
   <si>
     <t>little_car.obj</t>
   </si>
@@ -575,6 +575,24 @@
   </si>
   <si>
     <t>elte.png</t>
+  </si>
+  <si>
+    <t>Help 01</t>
+  </si>
+  <si>
+    <t>help_01.png</t>
+  </si>
+  <si>
+    <t>Help 02</t>
+  </si>
+  <si>
+    <t>Help 03</t>
+  </si>
+  <si>
+    <t>help_03.png</t>
+  </si>
+  <si>
+    <t>help_02.png</t>
   </si>
 </sst>
 </file>
@@ -1461,10 +1479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG38"/>
+  <dimension ref="A1:AG41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2489,23 +2507,23 @@
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A11" s="6">
-        <v>1</v>
+      <c r="A11" s="5">
+        <v>-1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>52</v>
+        <v>185</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>145</v>
+        <v>12</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>51</v>
+        <v>186</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>95</v>
+        <v>42</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>42</v>
@@ -2520,93 +2538,93 @@
         <v>42</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>175</v>
+        <v>42</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>142</v>
+        <v>42</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="V11" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="W11" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="Z11" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>122</v>
+        <v>42</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AD11" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AE11" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AF11" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AG11" s="1" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A12" s="7">
-        <v>2</v>
+      <c r="A12" s="5">
+        <v>-1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>146</v>
+        <v>187</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>145</v>
+        <v>12</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>147</v>
+        <v>190</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>42</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>148</v>
+        <v>42</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>42</v>
@@ -2621,93 +2639,93 @@
         <v>42</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>142</v>
+        <v>42</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>179</v>
+        <v>42</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="Z12" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="AB12" s="1" t="s">
-        <v>149</v>
+        <v>42</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AD12" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AE12" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AF12" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AG12" s="1" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A13" s="6">
-        <v>3</v>
+      <c r="A13" s="5">
+        <v>-1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>44</v>
+        <v>188</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>144</v>
+        <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>45</v>
+        <v>189</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>42</v>
@@ -2722,93 +2740,93 @@
         <v>42</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>112</v>
+        <v>42</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>111</v>
+        <v>42</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>111</v>
+        <v>42</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>111</v>
+        <v>42</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>142</v>
+        <v>42</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>141</v>
+        <v>42</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>111</v>
+        <v>42</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>105</v>
+        <v>42</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AD13" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AE13" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AF13" s="1" t="s">
-        <v>106</v>
+        <v>42</v>
       </c>
       <c r="AG13" s="1" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
-        <v>4</v>
+      <c r="A14" s="6">
+        <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>42</v>
@@ -2825,20 +2843,20 @@
       <c r="K14" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L14" s="2" t="s">
-        <v>112</v>
+      <c r="L14" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>105</v>
+        <v>175</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="Q14" s="1" t="s">
         <v>105</v>
@@ -2862,7 +2880,7 @@
         <v>105</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="Y14" s="1" t="s">
         <v>105</v>
@@ -2874,7 +2892,7 @@
         <v>105</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="AC14" s="1" t="s">
         <v>106</v>
@@ -2889,39 +2907,39 @@
         <v>106</v>
       </c>
       <c r="AG14" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A15" s="6">
-        <v>5</v>
+      <c r="A15" s="7">
+        <v>2</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>146</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1</v>
+        <v>145</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>129</v>
+        <v>42</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>4</v>
+        <v>42</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>5</v>
+        <v>42</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>105</v>
@@ -2963,19 +2981,19 @@
         <v>105</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y15" s="2" t="s">
-        <v>118</v>
+        <v>179</v>
+      </c>
+      <c r="Y15" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="AA15" s="1" t="s">
         <v>105</v>
       </c>
       <c r="AB15" s="1" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="AC15" s="1" t="s">
         <v>106</v>
@@ -2994,53 +3012,53 @@
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
-        <v>6</v>
+      <c r="A16" s="6">
+        <v>3</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>105</v>
+      <c r="L16" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>105</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="Q16" s="1" t="s">
         <v>105</v>
@@ -3064,19 +3082,19 @@
         <v>105</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y16" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="Y16" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="AA16" s="1" t="s">
         <v>105</v>
       </c>
       <c r="AB16" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="AC16" s="1" t="s">
         <v>106</v>
@@ -3095,53 +3113,53 @@
       </c>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A17" s="6">
-        <v>7</v>
+      <c r="A17" s="7">
+        <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1</v>
+        <v>144</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="K17" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>105</v>
+      <c r="L17" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>105</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="Q17" s="1" t="s">
         <v>105</v>
@@ -3165,19 +3183,19 @@
         <v>105</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y17" s="2" t="s">
-        <v>118</v>
+        <v>111</v>
+      </c>
+      <c r="Y17" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="Z17" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="AA17" s="1" t="s">
         <v>105</v>
       </c>
       <c r="AB17" s="1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="AC17" s="1" t="s">
         <v>106</v>
@@ -3192,39 +3210,39 @@
         <v>106</v>
       </c>
       <c r="AG17" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A18" s="7">
-        <v>8</v>
+      <c r="A18" s="6">
+        <v>5</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>53</v>
+        <v>2</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>105</v>
@@ -3257,7 +3275,7 @@
         <v>141</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>180</v>
+        <v>105</v>
       </c>
       <c r="V18" s="1" t="s">
         <v>105</v>
@@ -3268,8 +3286,8 @@
       <c r="X18" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="Y18" s="1" t="s">
-        <v>105</v>
+      <c r="Y18" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="Z18" s="1" t="s">
         <v>109</v>
@@ -3297,35 +3315,35 @@
       </c>
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A19" s="6">
-        <v>9</v>
+      <c r="A19" s="7">
+        <v>6</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>105</v>
@@ -3358,7 +3376,7 @@
         <v>141</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>180</v>
+        <v>105</v>
       </c>
       <c r="V19" s="1" t="s">
         <v>105</v>
@@ -3369,8 +3387,8 @@
       <c r="X19" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="Y19" s="1" t="s">
-        <v>105</v>
+      <c r="Y19" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="Z19" s="1" t="s">
         <v>109</v>
@@ -3398,35 +3416,35 @@
       </c>
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A20" s="7">
-        <v>10</v>
+      <c r="A20" s="6">
+        <v>7</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>105</v>
@@ -3459,7 +3477,7 @@
         <v>141</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>180</v>
+        <v>105</v>
       </c>
       <c r="V20" s="1" t="s">
         <v>105</v>
@@ -3470,8 +3488,8 @@
       <c r="X20" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="Y20" s="1" t="s">
-        <v>105</v>
+      <c r="Y20" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="Z20" s="1" t="s">
         <v>109</v>
@@ -3499,35 +3517,35 @@
       </c>
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A21" s="6">
-        <v>11</v>
+      <c r="A21" s="7">
+        <v>8</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>105</v>
@@ -3560,7 +3578,7 @@
         <v>141</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>105</v>
+        <v>180</v>
       </c>
       <c r="V21" s="1" t="s">
         <v>105</v>
@@ -3569,19 +3587,19 @@
         <v>105</v>
       </c>
       <c r="X21" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y21" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
+      </c>
+      <c r="Y21" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="Z21" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="AA21" s="1" t="s">
         <v>105</v>
       </c>
       <c r="AB21" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="AC21" s="1" t="s">
         <v>106</v>
@@ -3600,35 +3618,35 @@
       </c>
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A22" s="7">
-        <v>12</v>
+      <c r="A22" s="6">
+        <v>9</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>105</v>
@@ -3661,7 +3679,7 @@
         <v>141</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>105</v>
+        <v>180</v>
       </c>
       <c r="V22" s="1" t="s">
         <v>105</v>
@@ -3670,19 +3688,19 @@
         <v>105</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y22" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
+      </c>
+      <c r="Y22" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="Z22" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="AA22" s="1" t="s">
         <v>105</v>
       </c>
       <c r="AB22" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="AC22" s="1" t="s">
         <v>106</v>
@@ -3701,35 +3719,35 @@
       </c>
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A23" s="6">
-        <v>13</v>
+      <c r="A23" s="7">
+        <v>10</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>105</v>
@@ -3762,7 +3780,7 @@
         <v>141</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>105</v>
+        <v>180</v>
       </c>
       <c r="V23" s="1" t="s">
         <v>105</v>
@@ -3771,19 +3789,19 @@
         <v>105</v>
       </c>
       <c r="X23" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="Y23" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
+      </c>
+      <c r="Y23" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="Z23" s="1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="AA23" s="1" t="s">
         <v>105</v>
       </c>
       <c r="AB23" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="AC23" s="1" t="s">
         <v>106</v>
@@ -3802,35 +3820,35 @@
       </c>
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A24" s="7">
-        <v>14</v>
+      <c r="A24" s="6">
+        <v>11</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>105</v>
@@ -3874,11 +3892,11 @@
       <c r="X24" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="Y24" s="1" t="s">
-        <v>105</v>
+      <c r="Y24" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="Z24" s="1" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="AA24" s="1" t="s">
         <v>105</v>
@@ -3903,35 +3921,35 @@
       </c>
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A25" s="6">
-        <v>15</v>
+      <c r="A25" s="7">
+        <v>12</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>105</v>
@@ -3975,11 +3993,11 @@
       <c r="X25" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="Y25" s="1" t="s">
-        <v>105</v>
+      <c r="Y25" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="Z25" s="1" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="AA25" s="1" t="s">
         <v>105</v>
@@ -4004,35 +4022,35 @@
       </c>
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A26" s="7">
-        <v>16</v>
+      <c r="A26" s="6">
+        <v>13</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>105</v>
@@ -4076,11 +4094,11 @@
       <c r="X26" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="Y26" s="1" t="s">
-        <v>105</v>
+      <c r="Y26" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="Z26" s="1" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="AA26" s="1" t="s">
         <v>105</v>
@@ -4105,38 +4123,38 @@
       </c>
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A27" s="6">
-        <v>17</v>
+      <c r="A27" s="7">
+        <v>14</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>150</v>
+        <v>77</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>152</v>
+        <v>73</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>153</v>
+        <v>74</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>105</v>
@@ -4145,13 +4163,13 @@
         <v>105</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Q27" s="1" t="s">
         <v>105</v>
@@ -4175,19 +4193,19 @@
         <v>105</v>
       </c>
       <c r="X27" s="1" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
       <c r="Y27" s="1" t="s">
         <v>105</v>
       </c>
       <c r="Z27" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AA27" s="1" t="s">
         <v>105</v>
       </c>
       <c r="AB27" s="1" t="s">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="AC27" s="1" t="s">
         <v>106</v>
@@ -4206,38 +4224,38 @@
       </c>
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A28" s="7">
-        <v>18</v>
+      <c r="A28" s="6">
+        <v>15</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>151</v>
+        <v>78</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>152</v>
+        <v>73</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>154</v>
+        <v>76</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
       <c r="L28" s="1" t="s">
         <v>105</v>
@@ -4246,13 +4264,13 @@
         <v>105</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="Q28" s="1" t="s">
         <v>105</v>
@@ -4276,19 +4294,19 @@
         <v>105</v>
       </c>
       <c r="X28" s="1" t="s">
-        <v>149</v>
+        <v>119</v>
       </c>
       <c r="Y28" s="1" t="s">
         <v>105</v>
       </c>
       <c r="Z28" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AA28" s="1" t="s">
         <v>105</v>
       </c>
       <c r="AB28" s="1" t="s">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="AC28" s="1" t="s">
         <v>106</v>
@@ -4307,38 +4325,38 @@
       </c>
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A29" s="6">
-        <v>19</v>
+      <c r="A29" s="7">
+        <v>16</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>79</v>
+        <v>127</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>176</v>
+        <v>105</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>105</v>
@@ -4347,13 +4365,13 @@
         <v>105</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="P29" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="Q29" s="1" t="s">
         <v>105</v>
@@ -4377,19 +4395,19 @@
         <v>105</v>
       </c>
       <c r="X29" s="1" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="Y29" s="1" t="s">
         <v>105</v>
       </c>
       <c r="Z29" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AA29" s="1" t="s">
         <v>105</v>
       </c>
       <c r="AB29" s="1" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="AC29" s="1" t="s">
         <v>106</v>
@@ -4408,23 +4426,23 @@
       </c>
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A30" s="7">
-        <v>20</v>
+      <c r="A30" s="6">
+        <v>17</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>83</v>
+        <v>150</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>101</v>
+        <v>160</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>84</v>
+        <v>153</v>
       </c>
       <c r="G30" s="1" t="s">
         <v>42</v>
@@ -4448,13 +4466,13 @@
         <v>105</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O30" s="1" t="s">
         <v>108</v>
       </c>
       <c r="P30" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q30" s="1" t="s">
         <v>105</v>
@@ -4478,7 +4496,7 @@
         <v>105</v>
       </c>
       <c r="X30" s="1" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="Y30" s="1" t="s">
         <v>105</v>
@@ -4490,7 +4508,7 @@
         <v>105</v>
       </c>
       <c r="AB30" s="1" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="AC30" s="1" t="s">
         <v>106</v>
@@ -4509,23 +4527,23 @@
       </c>
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A31" s="6">
-        <v>21</v>
+      <c r="A31" s="7">
+        <v>18</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>85</v>
+        <v>151</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>86</v>
+        <v>152</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>102</v>
+        <v>161</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
       <c r="G31" s="1" t="s">
         <v>42</v>
@@ -4549,13 +4567,13 @@
         <v>105</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="O31" s="1" t="s">
         <v>108</v>
       </c>
       <c r="P31" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q31" s="1" t="s">
         <v>105</v>
@@ -4579,7 +4597,7 @@
         <v>105</v>
       </c>
       <c r="X31" s="1" t="s">
-        <v>111</v>
+        <v>149</v>
       </c>
       <c r="Y31" s="1" t="s">
         <v>105</v>
@@ -4591,7 +4609,7 @@
         <v>105</v>
       </c>
       <c r="AB31" s="1" t="s">
-        <v>106</v>
+        <v>149</v>
       </c>
       <c r="AC31" s="1" t="s">
         <v>106</v>
@@ -4610,23 +4628,23 @@
       </c>
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A32" s="7">
-        <v>22</v>
+      <c r="A32" s="6">
+        <v>19</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="G32" s="1" t="s">
         <v>42</v>
@@ -4711,23 +4729,23 @@
       </c>
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A33" s="6">
-        <v>23</v>
+      <c r="A33" s="7">
+        <v>20</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>42</v>
@@ -4812,23 +4830,23 @@
       </c>
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A34" s="7">
-        <v>24</v>
+      <c r="A34" s="6">
+        <v>21</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>60</v>
+        <v>85</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>61</v>
+        <v>86</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>42</v>
@@ -4852,13 +4870,13 @@
         <v>105</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>166</v>
+        <v>107</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>166</v>
+        <v>108</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>166</v>
+        <v>109</v>
       </c>
       <c r="Q34" s="1" t="s">
         <v>105</v>
@@ -4913,23 +4931,23 @@
       </c>
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A35" s="6">
-        <v>25</v>
+      <c r="A35" s="7">
+        <v>22</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>63</v>
+        <v>88</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>64</v>
+        <v>89</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>42</v>
@@ -4953,13 +4971,13 @@
         <v>105</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>171</v>
+        <v>107</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>171</v>
+        <v>109</v>
       </c>
       <c r="Q35" s="1" t="s">
         <v>105</v>
@@ -5014,23 +5032,23 @@
       </c>
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A36" s="7">
-        <v>26</v>
+      <c r="A36" s="6">
+        <v>23</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>159</v>
+        <v>91</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>155</v>
+        <v>92</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>167</v>
+        <v>104</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>162</v>
+        <v>93</v>
       </c>
       <c r="G36" s="1" t="s">
         <v>42</v>
@@ -5054,13 +5072,13 @@
         <v>105</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>171</v>
+        <v>107</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>171</v>
+        <v>109</v>
       </c>
       <c r="Q36" s="1" t="s">
         <v>105</v>
@@ -5115,23 +5133,23 @@
       </c>
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A37" s="6">
-        <v>27</v>
+      <c r="A37" s="7">
+        <v>24</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>157</v>
+        <v>60</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>156</v>
+        <v>61</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>168</v>
+        <v>96</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>163</v>
+        <v>62</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>42</v>
@@ -5155,13 +5173,13 @@
         <v>105</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="P37" s="1" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="Q37" s="1" t="s">
         <v>105</v>
@@ -5216,23 +5234,23 @@
       </c>
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A38" s="7">
-        <v>28</v>
+      <c r="A38" s="6">
+        <v>25</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>158</v>
+        <v>63</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>164</v>
+        <v>64</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>169</v>
+        <v>97</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>165</v>
+        <v>65</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>42</v>
@@ -5256,13 +5274,13 @@
         <v>105</v>
       </c>
       <c r="N38" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="P38" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="Q38" s="1" t="s">
         <v>105</v>
@@ -5313,6 +5331,309 @@
         <v>106</v>
       </c>
       <c r="AG38" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A39" s="7">
+        <v>26</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="O39" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="P39" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="R39" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="S39" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="T39" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="U39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="W39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="X39" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA39" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB39" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC39" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD39" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE39" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF39" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG39" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A40" s="6">
+        <v>27</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="O40" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="R40" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="S40" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="T40" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="U40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="W40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="X40" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF40" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG40" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="41" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A41" s="7">
+        <v>28</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="L41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N41" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="O41" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="P41" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="R41" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="S41" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="T41" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="U41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="V41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="W41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="X41" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AB41" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AC41" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD41" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE41" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF41" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AG41" s="1" t="s">
         <v>141</v>
       </c>
     </row>

</xml_diff>